<commit_message>
Update performance.py and Datasets
</commit_message>
<xml_diff>
--- a/Dataset/Best_XI.xlsx
+++ b/Dataset/Best_XI.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kecco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniDispense\ICON\ICON_Project\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867AA096-EE31-45DD-AED0-F18CF883C9CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15D123F-1C72-40ED-A58D-A77199FB1B51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="2208" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31470" yWindow="-5955" windowWidth="17850" windowHeight="14085" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="26" sheetId="1" r:id="rId1"/>
-    <sheet name="27" sheetId="2" r:id="rId2"/>
-    <sheet name="28" sheetId="3" r:id="rId3"/>
+    <sheet name="g26" sheetId="1" r:id="rId1"/>
+    <sheet name="g27" sheetId="2" r:id="rId2"/>
+    <sheet name="g28" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -479,20 +479,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -509,7 +509,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -526,7 +526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -543,7 +543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -560,7 +560,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -577,7 +577,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -594,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -611,7 +611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -645,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -662,7 +662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -679,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -696,7 +696,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <f>SUM(E2:E12)</f>
         <v>81.5</v>
@@ -712,19 +712,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BE4699-2264-4CD1-8D5C-BE6D7B0042CE}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -741,7 +741,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -758,7 +758,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -775,7 +775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -792,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -809,7 +809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -826,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -843,7 +843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -860,7 +860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -877,7 +877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -894,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -911,7 +911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -928,7 +928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <f>SUM(E2:E12)</f>
         <v>89.5</v>
@@ -944,18 +944,18 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -972,7 +972,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -989,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <f>SUM(E2:E12)</f>
         <v>79</v>

</xml_diff>